<commit_message>
added 3.3 and 3.4
</commit_message>
<xml_diff>
--- a/office/Zeitplan_Gr_G_Partyspot_Gubbauer_Haindl_Weghofer_v3.xlsx
+++ b/office/Zeitplan_Gr_G_Partyspot_Gubbauer_Haindl_Weghofer_v3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127F5E25-65B0-4927-837C-3C8699F79DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C6D18A-693C-45ED-A45D-297787A4DF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1957,7 +1957,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="39" fmlaLink="$J$2" max="110" min="1" page="10" val="39"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="39" fmlaLink="$J$2" max="110" min="1" page="10" val="42"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2249,7 +2249,7 @@
   <dimension ref="A1:DP47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2295,7 +2295,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="15">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="38" t="s">
@@ -3045,9 +3045,15 @@
       <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
+      <c r="G17" s="7">
+        <v>40</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+      <c r="I17" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
@@ -3066,9 +3072,15 @@
       <c r="F18" s="7">
         <v>4</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8"/>
+      <c r="G18" s="7">
+        <v>41</v>
+      </c>
+      <c r="H18" s="7">
+        <v>2</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="28" t="s">

</xml_diff>